<commit_message>
update excel template, data input (not finished)
</commit_message>
<xml_diff>
--- a/PPST/test_data_template.xlsx
+++ b/PPST/test_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicky\Desktop\Spring '25\SeniorProject\Senior-Project\PPST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E581ECB-2D55-4527-BB3B-8FBB213A584D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA5E268-C8B3-43D3-8310-2FD19F8A90B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Stimulus #</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Age</t>
-  </si>
-  <si>
-    <t>Response Time Per Click</t>
   </si>
   <si>
     <t>Stimuli</t>
@@ -101,6 +98,51 @@
   </si>
   <si>
     <t>Average Response Per Question</t>
+  </si>
+  <si>
+    <t>Response Char 1</t>
+  </si>
+  <si>
+    <t>Response Char 2</t>
+  </si>
+  <si>
+    <t>Response Char 3</t>
+  </si>
+  <si>
+    <t>Response Char 4</t>
+  </si>
+  <si>
+    <t>Response Char 5</t>
+  </si>
+  <si>
+    <t>Latency 1</t>
+  </si>
+  <si>
+    <t>Latency 2</t>
+  </si>
+  <si>
+    <t>Latency 4</t>
+  </si>
+  <si>
+    <t>Latency 3</t>
+  </si>
+  <si>
+    <t>Latency 5</t>
+  </si>
+  <si>
+    <t>Stimuli Char 1</t>
+  </si>
+  <si>
+    <t>Stimuli Char 2</t>
+  </si>
+  <si>
+    <t>Stimuli Char 3</t>
+  </si>
+  <si>
+    <t>Stimuli Char 4</t>
+  </si>
+  <si>
+    <t>Stimuli 5</t>
   </si>
 </sst>
 </file>
@@ -2087,16 +2129,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2124,15 +2166,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2445,24 +2487,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2481,21 +2529,65 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2514,10 +2606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD4744E-6ADD-47E4-B2D7-2A2A9E5E05EB}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,21 +2619,21 @@
     <col min="3" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" cm="1">
         <f t="array" ref="A2:A15">'Raw Data'!A5:A18</f>
         <v>0</v>
@@ -2550,117 +2642,332 @@
         <f t="array" ref="B2:B15">'Raw Data'!$C$5:'Raw Data'!$C$18='Raw Data'!$B$5:'Raw Data'!$B$18</f>
         <v>1</v>
       </c>
+      <c r="F2" t="str" cm="1">
+        <f t="array" ref="F2:J15">IF(
+  ( 'Raw Data'!D5:H18 &lt;&gt; "" ) * ( 'Raw Data'!A21:E34 &lt;&gt; "" ),
+  'Raw Data'!D5:H18 = 'Raw Data'!A21:E34,
+  ""
+)</f>
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more xl stuff, add search bar to test info
</commit_message>
<xml_diff>
--- a/PPST/test_data_template.xlsx
+++ b/PPST/test_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaslunt/Desktop/Spring '25/SeniorProject/Senior Project Repo/Senior-Project/PPST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicky\Desktop\Spring '25\SeniorProject\Senior-Project\PPST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223FD078-410A-7C49-9FB4-BF4E21EB0A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8908D07B-B139-4C27-8D5A-B6B38B815E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Stimulus #</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>Question Type</t>
-  </si>
-  <si>
-    <t>Average Response Per Click</t>
-  </si>
-  <si>
-    <t>Average Response Per Question</t>
   </si>
   <si>
     <t>Response Char 1</t>
@@ -202,12 +196,33 @@
   <si>
     <t>Avg. Char 5 Correctness</t>
   </si>
+  <si>
+    <t>Average Time Per Question</t>
+  </si>
+  <si>
+    <t>Average Latency Per Click</t>
+  </si>
+  <si>
+    <t>Avg. Char 2 Latency</t>
+  </si>
+  <si>
+    <t>Avg. Char 3 Latency</t>
+  </si>
+  <si>
+    <t>Avg. Char 4 Latency</t>
+  </si>
+  <si>
+    <t>Avg. Char 5 Latency</t>
+  </si>
+  <si>
+    <t>Avg. Char 1 Latency</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,6 +1142,682 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Latencies by Character</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Position</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Insights'!$F$20:$J$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Char 1 Latency</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg. Char 2 Latency</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Avg. Char 3 Latency</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Avg. Char 4 Latency</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Avg. Char 5 Latency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Insights'!$F$21:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D24-44AE-A8B2-2ED7AC026535}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="302021695"/>
+        <c:axId val="302022655"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="302021695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="302022655"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="302022655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latency (Seoncds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="302021695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Individual</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Character Average Correctness</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Insights'!$F$17:$J$17</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Char 1 Correctness</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg. Char 2 Correctness</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Avg. Char 3 Correctness</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Avg. Char 4 Correctness</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Avg. Char 5 Correctness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Insights'!$F$18:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6ECA-4053-900D-A9CA328FC626}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="309765583"/>
+        <c:axId val="309767503"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="309765583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="309767503"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="309767503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="309765583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1207,6 +1898,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2213,20 +2984,1030 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>638481</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>151997</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1313891</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333681</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>44583</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>299045</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>113856</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2253,16 +4034,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>260656</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>148822</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>814838</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>27595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>565456</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>41408</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>288366</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>110681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2282,6 +4063,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1316691</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>23531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>554691</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>99731</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F73861F0-10C9-5376-CC83-07214CCC0C5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>425824</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>77321</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404D938A-7679-6F37-0162-6BA98CA7885B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2577,26 +4430,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2615,7 +4470,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2626,54 +4481,54 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2692,26 +4547,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD4744E-6ADD-47E4-B2D7-2A2A9E5E05EB}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="4" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2725,25 +4580,25 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" cm="1">
         <f t="array" ref="A2:A15">'Raw Data'!A5:A18</f>
         <v>0</v>
@@ -2781,7 +4636,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2812,7 +4667,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2839,7 +4694,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2866,7 +4721,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2893,7 +4748,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2920,7 +4775,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2947,7 +4802,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2974,7 +4829,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3001,7 +4856,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3028,7 +4883,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3055,7 +4910,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3082,7 +4937,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3109,7 +4964,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3136,38 +4991,38 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="6">
         <f>IF(
   COUNTA(B4:B15)=0,
@@ -3184,7 +5039,7 @@
         <f>AVERAGE(D4:D15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F18" t="e">
+      <c r="F18" s="6" t="e">
         <f>IF(
   COUNTA(F4:F15)=0,
   "",
@@ -3192,7 +5047,7 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" t="e">
+      <c r="G18" s="6" t="e">
         <f t="shared" ref="G18:J18" si="1">IF(
   COUNTA(G4:G15)=0,
   "",
@@ -3200,16 +5055,55 @@
 )</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" t="e">
+      <c r="H18" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" t="e">
+      <c r="I18" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" t="e">
+      <c r="J18" s="6" t="e">
         <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="F20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="F21" t="e">
+        <f>AVERAGE('Raw Data'!I5:I18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" t="e">
+        <f>AVERAGE('Raw Data'!J5:J18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" t="e">
+        <f>AVERAGE('Raw Data'!K5:K18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f>AVERAGE('Raw Data'!L5:L18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" t="e">
+        <f>AVERAGE('Raw Data'!M5:M18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel can now handle all sized inputs
</commit_message>
<xml_diff>
--- a/PPST/test_data_template.xlsx
+++ b/PPST/test_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicky\Desktop\Spring '25\SeniorProject\Senior-Project\PPST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8908D07B-B139-4C27-8D5A-B6B38B815E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53624763-567E-40A3-99DF-3CEB3151E598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Stimulus #</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Avg. Char 1 Latency</t>
+  </si>
+  <si>
+    <t>Additional Chars</t>
   </si>
 </sst>
 </file>
@@ -4428,10 +4431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4441,17 +4444,17 @@
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="6" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4470,7 +4473,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -4496,21 +4499,24 @@
         <v>16</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4549,8 +4555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD4744E-6ADD-47E4-B2D7-2A2A9E5E05EB}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5087,23 +5093,23 @@
     </row>
     <row r="21" spans="1:10">
       <c r="F21" t="e">
-        <f>AVERAGE('Raw Data'!I5:I18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" t="e">
         <f>AVERAGE('Raw Data'!J5:J18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H21" t="e">
+      <c r="G21" t="e">
         <f>AVERAGE('Raw Data'!K5:K18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" t="e">
+      <c r="H21" t="e">
         <f>AVERAGE('Raw Data'!L5:L18)</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="I21" t="e">
+        <f>AVERAGE('Raw Data'!M5:M18)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="J21" t="e">
-        <f>AVERAGE('Raw Data'!M5:M18)</f>
+        <f>AVERAGE('Raw Data'!N5:N18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>